<commit_message>
updates in all lists and adding red, yellow, orange
</commit_message>
<xml_diff>
--- a/data/Eksklusion_lande/AP Pension_eksklusionsliste_lande_isin.xlsx
+++ b/data/Eksklusion_lande/AP Pension_eksklusionsliste_lande_isin.xlsx
@@ -136,7 +136,7 @@
     <t>Turkey</t>
   </si>
   <si>
-    <t>['XS1318576086', 'XS1819680288', 'XS1819680528', 'XS2083302419', 'XS2083302500', 'XS2446175577']</t>
+    <t>['XS1819680288', 'XS1819680528', 'XS2083302419', 'XS2083302500', 'XS2446175577']</t>
   </si>
   <si>
     <t>['XS1319820897', 'XS1678623734']</t>
@@ -145,7 +145,7 @@
     <t>['XS1110833123', 'XS2058948451', 'XS2172965282', 'XS2290957146', 'XS2290957732', 'XS2764424813', 'XS2834924867']</t>
   </si>
   <si>
-    <t>['XS1558078496', 'XS1775617464', 'XS1807305328', 'XS1953057061', 'XS1953057491', 'XS1980065301', 'XS1980255936', 'XS2053566068', 'XS2079842642', 'XS2176899701', 'XS2241075014', 'XS2297220423', 'XS2297221405', 'XS2297226545', 'XS2343007170', 'XS2391395154', 'XS2391398174', 'XS2530049837']</t>
+    <t>['XS1558078496', 'XS1775617464', 'XS1807305328', 'XS1953057061', 'XS1953057491', 'XS1980065301', 'XS1980255936', 'XS2079842642', 'XS2176899701', 'XS2241075014', 'XS2297220423', 'XS2297221405', 'XS2297226545', 'XS2391395154', 'XS2391398174', 'XS2530049837']</t>
   </si>
   <si>
     <t>['XS1151974877']</t>
@@ -178,7 +178,7 @@
     <t>['XS1717011982', 'XS1717013095', 'XS1777972941', 'XS1910826996', 'XS1910827887', 'XS1910828182', 'XS2337067792', 'XS2384701020', 'XS2384704800', 'XS2445169985']</t>
   </si>
   <si>
-    <t>['NO0011134405', 'RO1631DBN055', 'RO3B41D8EX14', 'RO4KELYFLVK4', 'RO7P95F9FNY6', 'ROGSHSTVFMX2', 'ROO7A2H5YIN8', 'US77586TAE64', 'XS1313004928', 'XS1405777589', 'XS1575967218', 'XS1575968026', 'XS1750113661', 'XS1750114396', 'XS1768074319', 'XS1837994794', 'XS1944412664', 'XS1944412748', 'XS1968706876', 'XS1970549561', 'XS2027596530', 'XS2109812508', 'XS2109813142', 'XS2178857954', 'XS2201851172', 'XS2201851685', 'XS2234859101', 'XS2248458395', 'XS2258400162', 'XS2262211076', 'XS2288906857', 'XS2310799809', 'XS2330503694', 'XS2330514899', 'XS2351310482', 'XS2364199757', 'XS2364200514', 'XS2434895558', 'XS2434895806', 'XS2434896010', 'XS2485249523', 'XS2571922884', 'XS2571923007', 'XS2571924070', 'XS2689095086', 'XS2689948078', 'XS2689949399', 'XS2756521212', 'XS2756521303', 'XS2770921315']</t>
+    <t>['XS1405777589', 'XS1575967218', 'XS1575968026', 'XS1750113661', 'XS1750114396', 'XS1944412664', 'XS1944412748', 'XS2234859101', 'XS2248458395', 'XS2288906857', 'XS2310799809', 'XS2351310482', 'XS2689095086']</t>
   </si>
   <si>
     <t>['XS1056560920', 'XS1729875598', 'XS2322319398', 'XS2322319638', 'XS2322321964', 'XS2348591707', 'XS2419405274']</t>
@@ -205,7 +205,7 @@
     <t>['XS0085134574']</t>
   </si>
   <si>
-    <t>['9.50% Angolan Government International Bond 2025', '8,25 ANGOL 09-05-2028 (REGS)', '8.25% Angolan Government International Bond 2028', 'REPUBLIC OF ANGOLA 8.25% 09.05.2028', 'REPUBLIC OF ANGOLA 9.375% 08.05.2048', 'REPUBLIC OF ANGOLA 8% 26.11.2029', '9,125 ANGOL 26-11-2049 (REGS)', 'REPUBLIC OF ANGOLA 9.125% 26.11.2049', '8,75 ANGOL 14-04-2032 (REGS)', '8.75% Angolan Government International Bond 2032', 'REPUBLIC OF ANGOLA 8.75% 14.04.2032']</t>
+    <t>['8,25 ANGOL 09-05-2028 (REGS)', 'REPUBLIC OF ANGOLA 8.25% 09.05.2028', 'REPUBLIC OF ANGOLA 9.375% 08.05.2048', 'REPUBLIC OF ANGOLA 8% 26.11.2029', '9,125 ANGOL 26-11-2049 (REGS)', 'REPUBLIC OF ANGOLA 9.125% 26.11.2049', '8,75 ANGOL 14-04-2032 (REGS)', 'REPUBLIC OF ANGOLA 8.75% 14.04.2032']</t>
   </si>
   <si>
     <t>['SOUTHERN GAS CORRIDOR 6.875% 24.03.2026', '3,5 AZERBJ 01-09-2032 (REGS)', 'REPUBLIC OF AZERBAIJAN 3.5% 01.09.2032']</t>
@@ -214,7 +214,7 @@
     <t>['KINGDOM OF BAHRAIN 6% 19.09.2044', '5,625 BHRAIN 30-09-2031 (REGS)', '7,375 BHRAIN 14-05-2030 (REGS)', '5,25 BHRAIN 25-01-2033 (REGS)', 'KINGDOM OF BAHRAIN 6.25% 25.01.2051', 'KINGDOM OF BAHRAIN 7.5% 12.02.2036', 'BANK BAHRAIN &amp; KUWAIT 6.875% 06.06.2029']</t>
   </si>
   <si>
-    <t>['ARAB REPUBLIC OF EGYPT 8.5% 31.01.2047', '7.90% Egypt Government International Bond 2048', 'ARAB REPUBLIC OF EGYPT 7.903% 21.02.2048', 'ARAB REPUBLIC OF EGYPT 5.625% 16.04.2030', 'ARAB REPUBLIC OF EGYPT 7.6003% 01.03.2029', '8.70% Egypt Government International Bond 2049', 'EGYPT 8.7002 03/01/49', 'ARAB REPUBLIC OF EGYPT 4.75% 11.04.2025', 'ARAB REPUBLIC OF EGYPT 6.375% 11.04.2031', 'EGYPT 6 3/8 04/11/31', 'AFRICAN EXPORT-IMPORT BA 3.994% 21.09.2029', 'ARAB REPUBLIC OF EGYPT 7.0529% 15.01.2032', '8,875 EGYPT 29-05-2050 (REGS)', 'ARAB REPUBLIC OF EGYPT 8.875% 29.05.2050', 'Egypt, Arab Republic Of (Government) 5.25% 20251006', 'ARAB REPUBLIC OF EGYPT 3.875% 16.02.2026', 'ARAB REPUBLIC OF EGYPT 7.5% 16.02.2061', '5,875 EGYPT 16-02-2031 (REGS)', '5.88% Egypt Government International Bond 2031', 'AFRICAN EXPORT-IMPORT BA 3.798% 17.05.2031', '7.30% Egypt Government International Bond 2033', '8.75% Egypt Government International Bond 2051', 'EGYPT 8 3/4 09/30/51', 'EGYPT TASKEEK CO 10.875% 28.02.2026', 'EGYPT TASKEEK COMPANY 10.875% 28.02.2026']</t>
+    <t>['ARAB REPUBLIC OF EGYPT 8.5% 31.01.2047', '7.90% Egypt Government International Bond 2048', 'ARAB REPUBLIC OF EGYPT 7.903% 21.02.2048', 'ARAB REPUBLIC OF EGYPT 5.625% 16.04.2030', 'ARAB REPUBLIC OF EGYPT 7.6003% 01.03.2029', '8.70% Egypt Government International Bond 2049', 'EGYPT 8.7002 03/01/49', 'ARAB REPUBLIC OF EGYPT 4.75% 11.04.2025', 'ARAB REPUBLIC OF EGYPT 6.375% 11.04.2031', 'EGYPT 6 3/8 04/11/31', 'ARAB REPUBLIC OF EGYPT 7.0529% 15.01.2032', '8,875 EGYPT 29-05-2050 (REGS)', 'ARAB REPUBLIC OF EGYPT 8.875% 29.05.2050', 'Egypt, Arab Republic Of (Government) 5.25% 20251006', 'ARAB REPUBLIC OF EGYPT 3.875% 16.02.2026', 'ARAB REPUBLIC OF EGYPT 7.5% 16.02.2061', '5,875 EGYPT 16-02-2031 (REGS)', '5.88% Egypt Government International Bond 2031', '7.30% Egypt Government International Bond 2033', '8.75% Egypt Government International Bond 2051', 'EGYPT 8 3/4 09/30/51', 'EGYPT TASKEEK CO 10.875% 28.02.2026', 'EGYPT TASKEEK COMPANY 10.875% 28.02.2026']</t>
   </si>
   <si>
     <t>['FEDERAL REP OF ETHIOPIA 11.12.2024']</t>
@@ -244,13 +244,13 @@
     <t>['Nigeria, Federal Republic Of (Government) 6.5% 20271128', 'Nigeria, Federal Republic Of (Government) 7.625% 20471128', 'REPUBLIC OF NIGERIA 7.625% 28.11.2047', 'Nigeria, Federal Republic Of (Government) 7.696% 20380223', '7.63% Nigeria Government International Bond 2025', 'Nigeria, Federal Republic Of (Government) 7.625% 20251121', '8.75% Nigeria Government International Bond 2031', 'Nigeria, Federal Republic Of (Government) 8.747% 20310121', 'REPUBLIC OF NIGERIA 8.747% 21.01.2031', 'Nigeria, Federal Republic Of (Government) 9.248% 20490121', 'AFRICA FINANCE CORP 2.875% 28.04.2028', '7,375 NGERIA 28-09-2033 (REGS)', 'REPUBLIC OF NIGERIA 7.375% 28.09.2033', '8,25 NGERIA 28-09-2051 (REGS)', 'Nigeria, Federal Republic Of (Government) 8.25% 20510928', 'REPUBLIC OF NIGERIA 8.25% 28.09.2051', '8,375 NGERIA 24-03-2029 (REGS)', '8.38% Nigeria Government International Bond 2029', 'Nigeria, Federal Republic Of (Government) 8.375% 20290324', 'REPUBLIC OF NIGERIA 8.375% 24.03.2029']</t>
   </si>
   <si>
-    <t>['14.02% Cidron Romanov Ltd 2026', 'ROMANIA GOVERNMENT BOND 3.65% 24.09.2031', 'ROMANIA GOVERNMENT BOND 4.85% 25.07.2029', '4,75 ROMGB 11-10-2034 (15Y)', 'ROMANIA GOVERNMENT BOND 2.5% 25.10.2027', '3,25 ROMGB 24-06-2026 (5Y)', 'ROMANIA GOVERNMENT BOND 6.7% 25.02.2032', 'Romania, Republic Of (Government) 6.125% 20440122', 'ROMANI 3 7/8 10/29/35', 'Romanian Government International Bond', '4,75 OMAN 15-06-2026 (REGS)', '5.38% Oman Government International Bond 2027', '6,5 OMAN 08-03-2047 (REGS)', 'OMAN GOV INTERNTL BOND 6.5% 08.03.2047', '5.63% Oman Government International Bond 2028', '6,75 OMAN 17-01-2048 (REGS)', 'OMAN 6 3/4 01/17/48', 'OMAN GOV INTERNTL BOND 6.75% 17.01.2048', 'ROMANIA 3.375% 08.02.2038', 'Romania, Republic Of (Government) 5.125% 20480615', 'OMAN 4 7/8 02/01/25', '6 OMAN 01-08-2029 (REGS)', '6.00% Oman Government International Bond 2029', '4.63% Romanian Government International Bond 2049', 'ROMANI 3 1/2 04/03/34', 'Romania, Republic Of (Government) 2.124% 20310716', 'Romania, Republic Of (Government) 2% 20320128', 'ROMANIA 3.375% 28.01.2050', 'ROMANIA 3.624% 26.05.2030', '3.00% Romanian Government International Bond 2031', 'Romania, Republic Of (Government) 3% 20310214', '4 ROMANI 14-02-2051 (REGS)', '4.00% Romanian Government International Bond 2051', 'Romania, Republic Of (Government) 4% 20510214', '6.75% Oman Government International Bond 2027', 'OQ SAOC 5.125% 06.05.2028', 'ROMANIA 2.625% 02.12.2040', 'Romania, Republic Of (Government) 1.375% 20291202', 'OMAN GOV INTERNTL BOND 7% 25.01.2051', 'BANK MUSCAT SAOG 4.75% 17.03.2026', 'Romania (Government) 2% 20330414', 'ROMANIA 2.75% 14.04.2041', 'OMAN SOVEREIGN SUKUK 4.875% 15.06.2030', 'Romania (Government) 1.75% 20300713', 'ROMANIA 2.875% 13.04.2042', '2,125% Romania 20280307', '3.63% Romanian Government International Bond 2032', 'Romania (Government) 3.625% 20320327', 'ROMANI 6 05/25/34', 'Romania (Government) 6% 20340525', '6.63% Romanian Government International Bond 2028', 'Romania 28', '7.13% Romanian Government International Bond 2033', 'Romania (Government) 7.125% 20330117', 'Romania (Government) 7.625% 20530117', 'ROMANIA 7.625% 17.01.2053', 'EDO SUKUK LTD 5.875% 21.09.2033', 'ROMANIA 6.375% 18.09.2033', 'ROMANIA 5.5% 18.09.2028', '5,875 ROMANI 30-01-2029 (REGS)', '5.88% Romanian Government International Bond 2029', '6.38% Romanian Government International Bond 2034']</t>
+    <t>['4,75 OMAN 15-06-2026 (REGS)', '5.38% Oman Government International Bond 2027', '6,5 OMAN 08-03-2047 (REGS)', 'OMAN GOV INTERNTL BOND 6.5% 08.03.2047', '5.63% Oman Government International Bond 2028', '6,75 OMAN 17-01-2048 (REGS)', 'OMAN 6 3/4 01/17/48', 'OMAN GOV INTERNTL BOND 6.75% 17.01.2048', 'OMAN 4 7/8 02/01/25', '6 OMAN 01-08-2029 (REGS)', '6.00% Oman Government International Bond 2029', '6.75% Oman Government International Bond 2027', 'OQ SAOC 5.125% 06.05.2028', 'OMAN GOV INTERNTL BOND 7% 25.01.2051', 'BANK MUSCAT SAOG 4.75% 17.03.2026', 'OMAN SOVEREIGN SUKUK 4.875% 15.06.2030', 'EDO SUKUK LTD 5.875% 21.09.2033']</t>
   </si>
   <si>
     <t>['8.25% Pakistan Government International Bond 2024', 'ISLAMIC REP OF PAKISTAN 6.875% 05.12.2027', 'ISLAMIC REP OF PAKISTAN 6% 08.04.2026', 'ISLAMIC REP OF PAKISTAN 7.375% 08.04.2031', '8,875 PKSTAN 08-04-2051 (REGS)', 'ISLAMIC REP OF PAKISTAN 8.875% 08.04.2051', 'PAKISTAN WATER &amp; POWER 7.5% 04.06.2031', '7,95 PKSTAN 31-01-2029 (REGS)']</t>
   </si>
   <si>
-    <t>['3,25 QATAR 02-06-2026 (REGS)', '4,5 QATAR 23-04-2028 (REGS)', '5.10% Qatar Government International Bond 2048', 'STATE OF QATAR 5.103% 23.04.2048', 'STATE OF QATAR 4.817% 14.03.2049', 'STATE OF QATAR 3.4% 16.04.2025', '3,75 QATAR 16-04-2030 (REGS)', '4,4 QATAR 16-04-2050 (REGS)', 'STATE OF QATAR 4.4% 16.04.2050', '2,25 QPETRO 12-07-2031 (REGS)', 'QATAR ENERGY 2.25% 12.07.2031']</t>
+    <t>['3,25 QATAR 02-06-2026 (REGS)', '4,5 QATAR 23-04-2028 (REGS)', '5.10% Qatar Government International Bond 2048', 'STATE OF QATAR 5.103% 23.04.2048', 'STATE OF QATAR 4.817% 14.03.2049', 'STATE OF QATAR 3.4% 16.04.2025', '3,75 QATAR 16-04-2030 (REGS)', '4,4 QATAR 16-04-2050 (REGS)', 'STATE OF QATAR 4.4% 16.04.2050', 'QATAR ENERGY 2.25% 12.07.2031']</t>
   </si>
   <si>
     <t>['5,5 RWANDA 09-08-2031 (REGS)', '5.50% Rwanda International Government Bond 2031', 'REPUBLIC OF RWANDA 5.5% 09.08.2031']</t>
@@ -271,7 +271,7 @@
     <t>['VIETNM Float 03/13/28']</t>
   </si>
   <si>
-    <t>['9.50% Angolan Government International Bond 2025', 'Angolan Government International Bond', 'Republic of Angola', '8.25% Angolan Government International Bond 2028', 'Angola', 'REPUBLIC OF ANGOLA  ', '8.75% Angolan Government International Bond 2032']</t>
+    <t>['Republic of Angola', 'Angola', 'Angolan Government International Bond', 'REPUBLIC OF ANGOLA  ']</t>
   </si>
   <si>
     <t>['Azerbaijan', 'Republic of Azerbaijan', 'REPUBLIC OF AZERBAIJAN  ']</t>
@@ -310,13 +310,13 @@
     <t>['NIGERIA, FEDERAL REPUBLIC OF (GOVERNMENT)', 'Nigeria', 'Nigeria Government International Bond', 'REPUBLIC OF NIGERIA  ', '7.63% Nigeria Government International Bond 2025', '8.75% Nigeria Government International Bond 2031', 'Federal Republic of Nigeria', '8.38% Nigeria Government International Bond 2029']</t>
   </si>
   <si>
-    <t>[nan, 'Romania Government Bond', 'Rumænien', 'Romania', 'ROMANIA (GOVERNMENT)', 'Romanian Gov.Int. Bond 29.10.2035', 'Romanian Gov.Int. Obligation 29.10.2035', 'Sultanate of Oman', '5.38% Oman Government International Bond 2027', 'Oman Government International Bond', 'Oman', 'OMAN GOV INTERNTL BOND  ', '5.63% Oman Government International Bond 2028', 'Oman Government International Bond 17.01.2048', 'Oman Government International Obligation 17.01.2048', 'ROMANIA  ', 'Romanian Government International Bond', 'Oman Government International Bond 01.02.2025', 'Oman Government International Obligation 01.02.2025', '6.00% Oman Government International Bond 2029', '4.63% Romanian Government International Bond 2049', 'Romanian Government International Bond 03.04.2034', 'Romanian Government International Obligation 03.04.2034', '3.00% Romanian Government International Bond 2031', '4.00% Romanian Government International Bond 2051', '6.75% Oman Government International Bond 2027', 'OMAN SOVEREIGN SUKUK  ', 'Oman Sovereign Sukuk Co', '3.63% Romanian Government International Bond 2032', 'Romanian Government International Bond 25.05.2034', 'Romanian Government International Obligation 25.05.2034', '6.63% Romanian Government International Bond 2028', 'Romania 28', '7.13% Romanian Government International Bond 2033', '5.88% Romanian Government International Bond 2029', '6.38% Romanian Government International Bond 2034']</t>
+    <t>['Sultanate of Oman', '5.38% Oman Government International Bond 2027', 'Oman Government International Bond', 'Oman', 'OMAN GOV INTERNTL BOND  ', '5.63% Oman Government International Bond 2028', 'Oman Government International Bond 17.01.2048', 'Oman Government International Obligation 17.01.2048', 'Oman Government International Bond 01.02.2025', 'Oman Government International Obligation 01.02.2025', '6.00% Oman Government International Bond 2029', '6.75% Oman Government International Bond 2027', 'OMAN SOVEREIGN SUKUK  ', 'Oman Sovereign Sukuk Co']</t>
   </si>
   <si>
     <t>['8.25% Pakistan Government International Bond 2024', 'ISLAMIC REP OF PAKISTAN  ', 'Pakistan', 'Pakistan Government International Bond', 'Islamic Republic of Pakistan', 'PAKISTAN WATER &amp; POWER  ', 'Pakistan Water &amp; Power Development Authority']</t>
   </si>
   <si>
-    <t>['State of Qatar', '5.10% Qatar Government International Bond 2048', 'Qatar Government International Bond', 'Qatar', 'STATE OF QATAR  ', 'QatarEnergy', 'QATAR ENERGY  ']</t>
+    <t>['State of Qatar', '5.10% Qatar Government International Bond 2048', 'Qatar Government International Bond', 'Qatar', 'STATE OF QATAR  ', 'QATAR ENERGY  ', 'QatarEnergy']</t>
   </si>
   <si>
     <t>['Republic of Rwanda', '5.50% Rwanda International Government Bond 2031', 'Rwanda International Government Bond', 'REPUBLIC OF RWANDA  ', 'Rwanda']</t>
@@ -337,7 +337,7 @@
     <t>['Vietnam 13.03.2028']</t>
   </si>
   <si>
-    <t>['Ringkøbing-Skjern', 'Region Nordjylland', 'Herning', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen']</t>
+    <t>['Herning', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen']</t>
   </si>
   <si>
     <t>['Fanø', 'Kalundborg', 'Herning']</t>
@@ -376,7 +376,7 @@
     <t>['Vesthimmerland', 'Fanø', 'Kalundborg', 'Rødovre', 'Vejen', 'Ringkøbing-Skjern', 'Region Nordjylland', 'Herning']</t>
   </si>
   <si>
-    <t>['Skive', 'Vejen', 'Kalundborg', 'Herning', 'Silkeborg', 'Vesthimmerland', 'Greve', 'Kolding', 'Fredericia', 'Hillerød', 'Lemvig', 'Varde', 'Aabenraa', 'Hedensted', 'Slagelse', 'Ringkøbing-Skjern', 'Region Nordjylland', 'Rødovre', 'Fanø', 'Vejle', 'Region Sjælland']</t>
+    <t>['Herning', 'Ringkøbing-Skjern', 'Region Nordjylland', 'Kalundborg', 'Rødovre', 'Vejen', 'Greve', 'Kolding', 'Skive', 'Fredericia', 'Hillerød', 'Lemvig', 'Varde', 'Aabenraa', 'Fanø']</t>
   </si>
   <si>
     <t>['Ringkøbing-Skjern', 'Kalundborg', 'Fanø', 'Rødovre', 'Vejen', 'Herning']</t>

</xml_diff>